<commit_message>
Correções feitas no Desafio HROADS
</commit_message>
<xml_diff>
--- a/DesafioHROADS/ModelagemFisicaHROADS.xlsx
+++ b/DesafioHROADS/ModelagemFisicaHROADS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitor Manoel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitor Manoel\OneDrive\Área de Trabalho\Sprint-1_BD_Relacional\DesafioHROADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D83725F9-D09C-4AA7-979A-6A7045FB1C51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{424E145B-512D-4560-AEEF-C771D56D9AD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A19C9796-FF3D-4FDC-8DB3-589F25059702}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Classe</t>
   </si>
@@ -120,14 +120,25 @@
   </si>
   <si>
     <t>Magia</t>
+  </si>
+  <si>
+    <t>ClasseHabilidade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -219,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -243,6 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6655A524-FF78-407C-8533-B991C85AD60D}">
-  <dimension ref="C2:N14"/>
+  <dimension ref="C2:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +585,7 @@
     <col min="9" max="9" width="12.140625" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" customWidth="1"/>
     <col min="13" max="13" width="15.28515625" customWidth="1"/>
     <col min="14" max="14" width="14.5703125" customWidth="1"/>
   </cols>
@@ -754,6 +766,10 @@
         <v>23</v>
       </c>
       <c r="I9" s="10"/>
+      <c r="K9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" s="10"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10" s="6" t="s">
@@ -771,6 +787,12 @@
       <c r="I10" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="K10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
@@ -788,6 +810,12 @@
       <c r="I11" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
@@ -805,6 +833,12 @@
       <c r="I12" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="K12" s="2">
+        <v>2</v>
+      </c>
+      <c r="L12" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
@@ -821,6 +855,12 @@
       </c>
       <c r="I13" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="K13" s="2">
+        <v>3</v>
+      </c>
+      <c r="L13" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.25">
@@ -831,13 +871,18 @@
         <v>28</v>
       </c>
     </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="M16" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="H2:N2"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="H9:I9"/>
+    <mergeCell ref="K9:L9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>